<commit_message>
Fix wrong column in sample XLSX file
</commit_message>
<xml_diff>
--- a/video/webapp/public/schedule_ex_de.xlsx
+++ b/video/webapp/public/schedule_ex_de.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Room ID</t>
   </si>
   <si>
-    <t xml:space="preserve">External URL</t>
+    <t xml:space="preserve">URL</t>
   </si>
   <si>
     <t xml:space="preserve">Beispiel</t>
@@ -463,12 +463,10 @@
   <dimension ref="A1:N1015"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.34"/>
@@ -3683,7 +3681,7 @@
       <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.14"/>
@@ -3790,7 +3788,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="54.64"/>
@@ -3876,7 +3874,7 @@
       <selection pane="bottomLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.55"/>

</xml_diff>